<commit_message>
Actividadesdel detalle de CP's
</commit_message>
<xml_diff>
--- a/ejemplos_clase/Facebook_Friend_Search_Scenario.xlsx
+++ b/ejemplos_clase/Facebook_Friend_Search_Scenario.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caryj\Documents\Curso Selenium\intro_automation-master\ejemplos_clase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CaroRB\repo\intro_automation\ejemplos_clase\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>ID</t>
   </si>
@@ -86,26 +86,35 @@
     <t>clic en botón buscar</t>
   </si>
   <si>
-    <t>Se muestran los resultados de las personas que tienen el mismo nombre</t>
-  </si>
-  <si>
     <t>omar navarro</t>
   </si>
   <si>
     <t>Búsqueda de amigo en Facebook</t>
+  </si>
+  <si>
+    <t>***********</t>
+  </si>
+  <si>
+    <t>Se muestran los resultados de las personas que tienen el nombre buscado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Ubuntu"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Ubuntu"/>
@@ -144,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -164,6 +173,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,7 +457,7 @@
   <dimension ref="A1:G1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -482,7 +492,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>8</v>
@@ -582,7 +592,9 @@
       <c r="C9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="5"/>
+      <c r="D9" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -611,7 +623,7 @@
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -625,7 +637,7 @@
         <v>20</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="2"/>
@@ -634,7 +646,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="9"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -9537,5 +9549,6 @@
     <hyperlink ref="D8" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>